<commit_message>
Mixed sample reversibilities implemented. Uses general only for promiscuous enzymes with shared steps
</commit_message>
<xml_diff>
--- a/input_test/HMP1489_r1_t0_profile.xlsx
+++ b/input_test/HMP1489_r1_t0_profile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="122">
   <si>
     <t>General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -385,7 +385,7 @@
     <t>Serotonin N-acetyltransferase is a monomeric enzyme (metacyc)</t>
   </si>
   <si>
-    <t>orderedBiBi</t>
+    <t>randomBiBiCompInhib</t>
   </si>
   <si>
     <t>ASMT has a C-terminal domain similar to other SAM-dependent O-methyltransferases, and an N-terminal domain which intertwines with another monomer to form the physiologically active dimer  (metacyc); inhib by melatonin</t>
@@ -517,7 +517,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="5:5 B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -653,7 +653,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="5:5 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -748,7 +748,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="5:5 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -929,7 +929,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="5:5 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1208,14 +1208,14 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="5:5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.9554655870445"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0931174089069"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1332,6 +1332,9 @@
       </c>
       <c r="B5" s="0" t="s">
         <v>117</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>0</v>
@@ -1476,7 +1479,7 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="5:5 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2119,7 +2122,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="5:5 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2452,7 +2455,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="5:5 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2633,7 +2636,7 @@
   <dimension ref="A2:A12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="5:5 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2715,7 +2718,7 @@
   <dimension ref="A2:A19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="5:5 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2832,7 +2835,7 @@
   <dimension ref="A2:A19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="5:5 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2949,7 +2952,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="5:5 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3097,7 +3100,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="5:5 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>